<commit_message>
feat: add Unidad de venta descripciones
</commit_message>
<xml_diff>
--- a/public/archivos/formato_carga_masiva_productos_tapices.xlsx
+++ b/public/archivos/formato_carga_masiva_productos_tapices.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ferna\Desktop\789.mx\Intercorp\public\archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE28AA2-602A-4D2C-8356-183514093F0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3A05269-0FA9-4755-AB2E-75C1C1DB7477}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Clave</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>Repeat HV</t>
+  </si>
+  <si>
+    <t>Unidad de medida</t>
   </si>
 </sst>
 </file>
@@ -1323,10 +1326,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:R2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="19.95" customHeight="1"/>
@@ -1348,11 +1351,12 @@
     <col min="15" max="15" width="15.21875" style="1" customWidth="1"/>
     <col min="16" max="16" width="13.33203125" style="1" customWidth="1"/>
     <col min="17" max="17" width="13.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="16384" width="8.33203125" style="1"/>
+    <col min="18" max="18" width="13.88671875" style="1" customWidth="1"/>
+    <col min="19" max="19" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="8.33203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="27.6" customHeight="1">
+    <row r="1" spans="1:19" ht="27.6" customHeight="1">
       <c r="A1" s="5" t="s">
         <v>16</v>
       </c>
@@ -1372,7 +1376,7 @@
       <c r="O1" s="5"/>
       <c r="P1" s="5"/>
     </row>
-    <row r="2" spans="1:18" ht="20.100000000000001" customHeight="1">
+    <row r="2" spans="1:19" ht="20.100000000000001" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -1425,6 +1429,9 @@
         <v>12</v>
       </c>
       <c r="R2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="S2" s="4" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>